<commit_message>
Files ready for production
Going to panelise seperate files to reduce PCBA cost
</commit_message>
<xml_diff>
--- a/PartsList.xlsx
+++ b/PartsList.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matja\Documents\Projects\TheFalcon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matja\Documents\Projects\PCBs\Keyboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16347EBC-F739-4F6E-9465-64C1772E66FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE310610-1642-4D72-94A3-B1FD26362629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{FE2F31EC-1493-4486-83E7-300EEFA8040E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="3" xr2:uid="{FE2F31EC-1493-4486-83E7-300EEFA8040E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="JLCPCB(Detailed)" sheetId="3" r:id="rId3"/>
-    <sheet name="SA_Retail" sheetId="4" r:id="rId4"/>
+    <sheet name="Left" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="231">
   <si>
     <t>Name</t>
   </si>
@@ -215,9 +215,6 @@
     <t>22u</t>
   </si>
   <si>
-    <t>0,1u</t>
-  </si>
-  <si>
     <t>100n</t>
   </si>
   <si>
@@ -242,9 +239,6 @@
     <t>10k</t>
   </si>
   <si>
-    <t>2k</t>
-  </si>
-  <si>
     <t>1k5</t>
   </si>
   <si>
@@ -266,9 +260,6 @@
     <t>Push Button</t>
   </si>
   <si>
-    <t>Switch</t>
-  </si>
-  <si>
     <t>STM32</t>
   </si>
   <si>
@@ -480,6 +471,267 @@
   </si>
   <si>
     <t>Rubber feet</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/18426-UNI_ROYAL0805W8F510JT5E/C17738</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Designator</t>
+  </si>
+  <si>
+    <t>Footprint</t>
+  </si>
+  <si>
+    <t>LCSC Part Number</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD:C_0402_1005Metric</t>
+  </si>
+  <si>
+    <t>C1524</t>
+  </si>
+  <si>
+    <t>C2,C3,C4,C5,C8,C9,C12,C14</t>
+  </si>
+  <si>
+    <t>C1525</t>
+  </si>
+  <si>
+    <t>C15,C16</t>
+  </si>
+  <si>
+    <t>C1545</t>
+  </si>
+  <si>
+    <t>C7,C13,C17</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD:C_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>C1592</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD:C_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>C1713</t>
+  </si>
+  <si>
+    <t>C10,C11</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD:C_1206_3216Metric</t>
+  </si>
+  <si>
+    <t>C1859</t>
+  </si>
+  <si>
+    <t>D1,D2,D3,D4,D5,D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,D19,D20,D21,D22,D23,D24,D25,D26,D27,D28,D29,D30,D31,D32,D33,D36,D37,D38</t>
+  </si>
+  <si>
+    <t>Diode_SMD:D_SOD-123</t>
+  </si>
+  <si>
+    <t>C2099</t>
+  </si>
+  <si>
+    <t>AMS1117-3.3</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>Package_TO_SOT_SMD:SOT-223-3_TabPin2</t>
+  </si>
+  <si>
+    <t>C6186</t>
+  </si>
+  <si>
+    <t>X322516MOB4SI</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>SamacSys_Parts:X322516MOB4SI</t>
+  </si>
+  <si>
+    <t>C12668</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>Resistor_SMD:R_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>C14675</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>C15401</t>
+  </si>
+  <si>
+    <t>R11,R13,R16,R19,R22</t>
+  </si>
+  <si>
+    <t>C17738</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>C22843</t>
+  </si>
+  <si>
+    <t>R9,R10,R12,R14,R15,R17,R18,R20,R21,R23</t>
+  </si>
+  <si>
+    <t>C22950</t>
+  </si>
+  <si>
+    <t>5k1</t>
+  </si>
+  <si>
+    <t>R1,R2,R3,R4</t>
+  </si>
+  <si>
+    <t>C23067</t>
+  </si>
+  <si>
+    <t>R24,R33</t>
+  </si>
+  <si>
+    <t>C23162</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>D39</t>
+  </si>
+  <si>
+    <t>LED_SMD:LED_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>C84260</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Fuse:Fuse_1206_3216Metric</t>
+  </si>
+  <si>
+    <t>C135336</t>
+  </si>
+  <si>
+    <t>SW_Push</t>
+  </si>
+  <si>
+    <t>SW1,SW2</t>
+  </si>
+  <si>
+    <t>Button_Switch_SMD:SW_SPST_B3U-1000P</t>
+  </si>
+  <si>
+    <t>C231329</t>
+  </si>
+  <si>
+    <t>STM32G431CBTx</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>Package_QFP:LQFP-48_7x7mm_P0.5mm</t>
+  </si>
+  <si>
+    <t>C529355</t>
+  </si>
+  <si>
+    <t>IS31FL3729-QFLS4-TR</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>SamacSys_Parts:QFN40P400X400X80-33N-D</t>
+  </si>
+  <si>
+    <t>C2940549</t>
+  </si>
+  <si>
+    <t>USB_C_Receptacle_USB2.0_16P</t>
+  </si>
+  <si>
+    <t>USB1,USB2</t>
+  </si>
+  <si>
+    <t>Connector_USB:USB_C_Receptacle_G-Switch_GT-USB-7010ASV</t>
+  </si>
+  <si>
+    <t>C2988369</t>
+  </si>
+  <si>
+    <t>U2,U3</t>
+  </si>
+  <si>
+    <t>Package_TO_SOT_SMD:SOT-666</t>
+  </si>
+  <si>
+    <t>C29780639</t>
+  </si>
+  <si>
+    <t>Extended</t>
+  </si>
+  <si>
+    <t>New Part Number</t>
+  </si>
+  <si>
+    <t>C15850</t>
+  </si>
+  <si>
+    <t>C15195</t>
+  </si>
+  <si>
+    <t>C15849</t>
+  </si>
+  <si>
+    <t>C12891</t>
+  </si>
+  <si>
+    <t>C32949</t>
+  </si>
+  <si>
+    <t>C23186</t>
+  </si>
+  <si>
+    <t>C25803</t>
+  </si>
+  <si>
+    <t>C25804</t>
+  </si>
+  <si>
+    <t>C84256</t>
+  </si>
+  <si>
+    <t>C81598</t>
+  </si>
+  <si>
+    <t>C720477</t>
   </si>
 </sst>
 </file>
@@ -913,24 +1165,24 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" customWidth="1"/>
-    <col min="6" max="6" width="24.88671875" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="21.33203125" customWidth="1"/>
-    <col min="9" max="9" width="25.5546875" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="22.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -980,7 +1232,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1029,7 +1281,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1078,7 +1330,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1121,7 +1373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1164,7 +1416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1213,7 +1465,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1256,7 +1508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1299,7 +1551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1342,7 +1594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1388,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1434,7 +1686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1480,7 +1732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1526,7 +1778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1572,7 +1824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1618,7 +1870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1647,12 +1899,12 @@
         <v>574.16039999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1660,7 +1912,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1668,7 +1920,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1676,7 +1928,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -1699,7 +1951,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -1721,7 +1973,7 @@
       </c>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1743,7 +1995,7 @@
       </c>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1765,7 +2017,7 @@
       </c>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -1787,7 +2039,7 @@
       </c>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -1817,7 +2069,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1839,7 +2091,7 @@
       </c>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1861,7 +2113,7 @@
       </c>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -1883,7 +2135,7 @@
       </c>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -1910,7 +2162,7 @@
       </c>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -1937,7 +2189,7 @@
       </c>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1964,7 +2216,7 @@
       </c>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C35">
         <f t="shared" si="9"/>
         <v>10</v>
@@ -1985,7 +2237,7 @@
       </c>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>29</v>
       </c>
@@ -2009,7 +2261,7 @@
       </c>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C37">
         <f t="shared" si="9"/>
         <v>10</v>
@@ -2030,7 +2282,7 @@
       </c>
       <c r="H37" s="4"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F39" s="4">
         <f>SUM(F24:F37)</f>
         <v>52.198343999999999</v>
@@ -2054,22 +2306,22 @@
       <selection sqref="A1:Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" customWidth="1"/>
-    <col min="17" max="17" width="9.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2113,7 +2365,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2171,7 +2423,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2217,7 +2469,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2266,7 +2518,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2315,7 +2567,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2364,7 +2616,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2407,7 +2659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2450,7 +2702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2493,7 +2745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2539,7 +2791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2585,7 +2837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -2631,7 +2883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2677,7 +2929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2723,7 +2975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -2769,7 +3021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -2809,7 +3061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2830,7 +3082,7 @@
         <v>942.07927999999993</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -2871,7 +3123,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2920,7 +3172,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -2963,7 +3215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -3006,7 +3258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -3049,7 +3301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -3095,7 +3347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -3138,7 +3390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -3181,7 +3433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -3224,7 +3476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -3270,7 +3522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -3316,7 +3568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -3362,7 +3614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -3408,7 +3660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -3454,7 +3706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>20</v>
       </c>
@@ -3500,7 +3752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -3509,7 +3761,7 @@
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -3539,34 +3791,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59C7F33A-CEE5-46B8-B073-2F922778444F}">
   <dimension ref="A1:T67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A13" sqref="A13"/>
-      <selection pane="topRight" activeCell="G49" sqref="G49"/>
+      <selection pane="topRight" activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" customWidth="1"/>
-    <col min="9" max="9" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.44140625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" style="5" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8" customWidth="1"/>
-    <col min="17" max="17" width="74.33203125" customWidth="1"/>
-    <col min="18" max="18" width="13.5546875" customWidth="1"/>
+    <col min="17" max="17" width="74.28515625" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3607,22 +3859,22 @@
         <v>23</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O1" t="s">
         <v>43</v>
       </c>
       <c r="Q1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="R1" t="s">
         <v>34</v>
       </c>
       <c r="T1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
@@ -3671,7 +3923,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="O2" t="s">
         <v>42</v>
@@ -3679,17 +3931,17 @@
       <c r="P2">
         <v>3</v>
       </c>
-      <c r="Q2" t="s">
-        <v>80</v>
+      <c r="Q2" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="T2" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="3">
         <v>8</v>
@@ -3733,19 +3985,19 @@
         <v>1</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="Q3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="T3" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -3789,16 +4041,16 @@
         <v>1</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="Q4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="T4" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="5" t="s">
         <v>56</v>
@@ -3845,16 +4097,16 @@
         <v>1</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="Q5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="T5" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="5" t="s">
         <v>57</v>
@@ -3901,19 +4153,19 @@
         <v>1</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="T6" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="3">
         <v>2</v>
@@ -3957,16 +4209,16 @@
         <v>1</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="T7" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C8" s="3">
         <f>SUM(C2:C7)</f>
         <v>17</v>
@@ -3977,16 +4229,13 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="T8" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" s="3">
         <v>4</v>
@@ -4030,22 +4279,22 @@
         <v>1</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="R9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="T9" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
@@ -4089,22 +4338,22 @@
         <v>1</v>
       </c>
       <c r="N10" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q10" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="Q10" s="6" t="s">
-        <v>87</v>
-      </c>
       <c r="R10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="T10" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -4148,22 +4397,22 @@
         <v>1</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="R11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="T11" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C12" s="3">
         <v>2</v>
@@ -4207,19 +4456,19 @@
         <v>1</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="R12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="T12" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="5">
         <v>20</v>
@@ -4266,16 +4515,16 @@
         <v>1</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="Q13" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T13" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="5">
         <v>51</v>
@@ -4322,19 +4571,19 @@
         <v>1</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="Q14" s="6" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="T14" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -4378,19 +4627,19 @@
         <v>1</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="Q15" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="T15" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
@@ -4434,16 +4683,16 @@
         <v>1</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="Q16" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="T16" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C17" s="3">
         <f>SUM(C9:C16)</f>
         <v>25</v>
@@ -4454,11 +4703,8 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-      <c r="T17" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -4507,18 +4753,18 @@
         <v>1</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="Q18" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="T18" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>42</v>
@@ -4565,21 +4811,21 @@
         <v>1</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="Q19" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="T19" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20" s="3">
         <v>1</v>
@@ -4623,21 +4869,21 @@
         <v>1</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="Q20" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="T20" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C21" s="3">
         <v>1</v>
@@ -4681,21 +4927,21 @@
         <v>1</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Q21" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="T21" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C22" s="3">
         <v>2</v>
@@ -4721,37 +4967,34 @@
       </c>
       <c r="I22" s="4">
         <f t="shared" si="5"/>
-        <v>2.08962</v>
+        <v>0</v>
       </c>
       <c r="J22" s="4">
         <f t="shared" si="8"/>
-        <v>4.1792400000000001</v>
+        <v>0</v>
       </c>
       <c r="K22" s="4">
         <f t="shared" si="9"/>
-        <v>12.53772</v>
+        <v>0</v>
       </c>
       <c r="L22" s="4">
         <f t="shared" si="10"/>
-        <v>20.8962</v>
+        <v>0</v>
       </c>
       <c r="M22" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q22" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="T22" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C23" s="3">
         <v>1</v>
@@ -4792,16 +5035,13 @@
         <v>0</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="T23" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C24" s="3">
         <v>1</v>
@@ -4842,21 +5082,18 @@
         <v>1</v>
       </c>
       <c r="R24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="S24" t="s">
-        <v>126</v>
-      </c>
-      <c r="T24" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C25" s="3">
         <v>38</v>
@@ -4900,7 +5137,7 @@
         <v>1</v>
       </c>
       <c r="Q25" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="R25" t="s">
         <v>52</v>
@@ -4909,9 +5146,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>42</v>
@@ -4958,9 +5195,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>42</v>
@@ -5007,18 +5244,18 @@
         <v>1</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="Q27" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="T27" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>42</v>
@@ -5065,15 +5302,15 @@
         <v>1</v>
       </c>
       <c r="Q28" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="T28" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>42</v>
@@ -5120,13 +5357,13 @@
         <v>1</v>
       </c>
       <c r="Q29" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="T29" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -5175,18 +5412,18 @@
         <v>1</v>
       </c>
       <c r="Q30" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="T30" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C31" s="3">
         <v>2</v>
@@ -5230,13 +5467,13 @@
         <v>1</v>
       </c>
       <c r="Q31" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="T31" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -5285,15 +5522,15 @@
         <v>1</v>
       </c>
       <c r="Q32" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="T32" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>42</v>
@@ -5336,13 +5573,10 @@
       <c r="M33" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="T33" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C34" s="3">
         <v>0</v>
@@ -5386,16 +5620,13 @@
       <c r="M34" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="T34" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C35" s="3">
         <v>0</v>
@@ -5439,102 +5670,99 @@
         <v>1</v>
       </c>
       <c r="Q35" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="T35" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C36" s="3">
         <f>C8+C17+SUM(C18:C34)</f>
         <v>178</v>
       </c>
       <c r="I36" s="4">
         <f>SUM(I2:I34)</f>
-        <v>127.495396</v>
+        <v>125.405776</v>
       </c>
       <c r="J36" s="4">
         <f t="shared" ref="J36:L36" si="20">SUM(J2:J34)</f>
-        <v>254.990792</v>
+        <v>250.81155200000001</v>
       </c>
       <c r="K36" s="4">
         <f t="shared" si="20"/>
-        <v>764.97237599999994</v>
+        <v>752.4346559999999</v>
       </c>
       <c r="L36" s="4">
         <f t="shared" si="20"/>
-        <v>1274.9539600000001</v>
-      </c>
-      <c r="T36" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+        <v>1254.0577599999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>133</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="K37" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>135</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="K37" t="s">
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>138</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>141</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>138</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>143</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>141</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>144</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>146</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>131</v>
-      </c>
       <c r="B44" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C45">
         <v>900</v>
       </c>
     </row>
-    <row r="53" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -5543,7 +5771,7 @@
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
     </row>
-    <row r="54" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
@@ -5552,7 +5780,7 @@
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
     </row>
-    <row r="55" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
@@ -5561,7 +5789,7 @@
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
     </row>
-    <row r="56" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
@@ -5570,7 +5798,7 @@
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
     </row>
-    <row r="57" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
@@ -5579,7 +5807,7 @@
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
     </row>
-    <row r="58" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
@@ -5588,7 +5816,7 @@
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
     </row>
-    <row r="59" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
@@ -5597,7 +5825,7 @@
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
     </row>
-    <row r="60" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -5606,7 +5834,7 @@
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
     </row>
-    <row r="61" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -5615,7 +5843,7 @@
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
     </row>
-    <row r="62" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -5624,7 +5852,7 @@
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
     </row>
-    <row r="63" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -5633,7 +5861,7 @@
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
     </row>
-    <row r="64" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -5642,7 +5870,7 @@
       <c r="K64" s="4"/>
       <c r="L64" s="4"/>
     </row>
-    <row r="65" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
@@ -5651,7 +5879,7 @@
       <c r="K65" s="4"/>
       <c r="L65" s="4"/>
     </row>
-    <row r="66" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -5660,7 +5888,7 @@
       <c r="K66" s="4"/>
       <c r="L66" s="4"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
       <c r="I67" s="4"/>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
@@ -5681,2093 +5909,586 @@
     <hyperlink ref="Q11" r:id="rId6" xr:uid="{EE9ED8F2-63F4-419C-BA79-711DF4C9CFCA}"/>
     <hyperlink ref="Q12" r:id="rId7" xr:uid="{E8228109-21DC-4AF0-8358-35DBB0A989AB}"/>
     <hyperlink ref="Q13" r:id="rId8" xr:uid="{AE79385F-DC7F-488B-B6A8-2C545215857B}"/>
-    <hyperlink ref="Q14" r:id="rId9" xr:uid="{C77B2309-46B8-4A9B-BFAA-0CE4179B9417}"/>
-    <hyperlink ref="Q15" r:id="rId10" xr:uid="{A326CC68-C8F5-4180-925B-17BB15FB43BE}"/>
-    <hyperlink ref="Q16" r:id="rId11" xr:uid="{0C2ABD71-670B-49BD-B6BE-2A22ED6BBD3F}"/>
-    <hyperlink ref="Q18" r:id="rId12" xr:uid="{FACE57B3-7BF1-4120-BFB7-737388D5DC5E}"/>
-    <hyperlink ref="Q19" r:id="rId13" xr:uid="{36CB7994-3DBF-42B4-9BB8-0255170FAF29}"/>
-    <hyperlink ref="Q20" r:id="rId14" xr:uid="{032466F2-8D68-4209-BA71-4ACBC3B77B0A}"/>
-    <hyperlink ref="Q21" r:id="rId15" xr:uid="{0967E55E-7F19-4FF3-97CF-42160684A56D}"/>
-    <hyperlink ref="Q22" r:id="rId16" xr:uid="{DAB5A52E-0755-4001-9C9E-09A525477A8E}"/>
-    <hyperlink ref="Q25" r:id="rId17" xr:uid="{C751D435-BB53-4EDD-B7BA-E962B522D0F8}"/>
-    <hyperlink ref="Q27" r:id="rId18" xr:uid="{72D56853-1E53-4D3D-9888-ACF3B09122A6}"/>
-    <hyperlink ref="Q28" r:id="rId19" xr:uid="{D3FA0264-5B24-4353-BC98-13DFE7E4FE74}"/>
-    <hyperlink ref="Q30" r:id="rId20" xr:uid="{2B274303-9C2A-412E-A03C-7AF1A049CC73}"/>
-    <hyperlink ref="Q31" r:id="rId21" xr:uid="{F07F664C-D317-4D1F-9E96-66A7787F3613}"/>
-    <hyperlink ref="Q32" r:id="rId22" xr:uid="{7533DF3D-4207-4BFF-BC01-4EAE17618D81}"/>
-    <hyperlink ref="Q35" r:id="rId23" xr:uid="{80F72AC2-BB4D-4239-9AD1-8E3C716C18EC}"/>
+    <hyperlink ref="Q15" r:id="rId9" xr:uid="{A326CC68-C8F5-4180-925B-17BB15FB43BE}"/>
+    <hyperlink ref="Q16" r:id="rId10" xr:uid="{0C2ABD71-670B-49BD-B6BE-2A22ED6BBD3F}"/>
+    <hyperlink ref="Q18" r:id="rId11" xr:uid="{FACE57B3-7BF1-4120-BFB7-737388D5DC5E}"/>
+    <hyperlink ref="Q19" r:id="rId12" xr:uid="{36CB7994-3DBF-42B4-9BB8-0255170FAF29}"/>
+    <hyperlink ref="Q20" r:id="rId13" xr:uid="{032466F2-8D68-4209-BA71-4ACBC3B77B0A}"/>
+    <hyperlink ref="Q21" r:id="rId14" xr:uid="{0967E55E-7F19-4FF3-97CF-42160684A56D}"/>
+    <hyperlink ref="Q22" r:id="rId15" xr:uid="{DAB5A52E-0755-4001-9C9E-09A525477A8E}"/>
+    <hyperlink ref="Q25" r:id="rId16" xr:uid="{C751D435-BB53-4EDD-B7BA-E962B522D0F8}"/>
+    <hyperlink ref="Q27" r:id="rId17" xr:uid="{72D56853-1E53-4D3D-9888-ACF3B09122A6}"/>
+    <hyperlink ref="Q28" r:id="rId18" xr:uid="{D3FA0264-5B24-4353-BC98-13DFE7E4FE74}"/>
+    <hyperlink ref="Q30" r:id="rId19" xr:uid="{2B274303-9C2A-412E-A03C-7AF1A049CC73}"/>
+    <hyperlink ref="Q31" r:id="rId20" xr:uid="{F07F664C-D317-4D1F-9E96-66A7787F3613}"/>
+    <hyperlink ref="Q32" r:id="rId21" xr:uid="{7533DF3D-4207-4BFF-BC01-4EAE17618D81}"/>
+    <hyperlink ref="Q35" r:id="rId22" xr:uid="{80F72AC2-BB4D-4239-9AD1-8E3C716C18EC}"/>
+    <hyperlink ref="Q2" r:id="rId23" xr:uid="{5E5203B7-C947-4C0A-AC9E-1C0513F96C86}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E754D4-4516-4302-9C86-DDB3C979809C}">
-  <dimension ref="A1:S63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04496EBE-FF58-4432-A51C-6782192DBBAD}">
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.109375" customWidth="1"/>
-    <col min="17" max="17" width="4.33203125" customWidth="1"/>
-    <col min="18" max="18" width="19.6640625" customWidth="1"/>
-    <col min="19" max="19" width="54.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>54</v>
+        <v>145</v>
+      </c>
+      <c r="B1" t="s">
+        <v>146</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>147</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>148</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>218</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" t="s">
-        <v>45</v>
+        <v>219</v>
       </c>
       <c r="H1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L1" t="s">
-        <v>49</v>
-      </c>
-      <c r="M1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R1" t="s">
-        <v>79</v>
-      </c>
-      <c r="S1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H2" t="str">
+        <f>IF(E2,F2,D2)</f>
+        <v>C15195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H24" si="0">IF(E3,F3,D3)</f>
+        <v>C1525</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>C32949</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>C15849</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3">
-        <f t="shared" ref="D2:D31" si="0">2*C2</f>
-        <v>2</v>
-      </c>
-      <c r="E2" s="3">
-        <f t="shared" ref="E2:E31" si="1">D2*$P$2</f>
-        <v>6</v>
-      </c>
-      <c r="F2">
-        <f>D2*5</f>
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>0.1</v>
-      </c>
-      <c r="H2">
-        <f>G2*17.86</f>
-        <v>1.786</v>
-      </c>
-      <c r="I2" s="4">
-        <f>IF($M2, $H2*C2, 0)</f>
-        <v>1.786</v>
-      </c>
-      <c r="J2" s="4">
-        <f t="shared" ref="J2:L16" si="2">IF($M2, $H2*D2, 0)</f>
-        <v>3.5720000000000001</v>
-      </c>
-      <c r="K2" s="4">
-        <f t="shared" si="2"/>
-        <v>10.716000000000001</v>
-      </c>
-      <c r="L2" s="4">
-        <f t="shared" si="2"/>
-        <v>17.86</v>
-      </c>
-      <c r="M2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="O2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P2">
-        <v>3</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>53</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="B6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>C15850</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" t="s">
+        <v>164</v>
+      </c>
+      <c r="E7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>C12891</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" t="s">
+        <v>167</v>
+      </c>
+      <c r="E8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>C81598</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>C6186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C10" t="s">
+        <v>174</v>
+      </c>
+      <c r="D10" t="s">
+        <v>175</v>
+      </c>
+      <c r="E10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>C12668</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" t="s">
+        <v>177</v>
+      </c>
+      <c r="D11" t="s">
+        <v>178</v>
+      </c>
+      <c r="E11" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>C25803</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C12" t="s">
+        <v>177</v>
+      </c>
+      <c r="D12" t="s">
+        <v>180</v>
+      </c>
+      <c r="E12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>C25804</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="3">
-        <v>4</v>
-      </c>
-      <c r="D3" s="3">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E3" s="3">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F31" si="3">D3*5</f>
-        <v>40</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H31" si="4">G3*17.86</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="4">
-        <f t="shared" ref="I3:L31" si="5">IF($M3, $H3*C3, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="J3" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K3" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L3" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M3" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E4" s="3">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I4" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J4" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K4" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M4" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E5" s="3">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="3"/>
+      <c r="B13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C13" t="s">
+        <v>177</v>
+      </c>
+      <c r="D13" t="s">
+        <v>182</v>
+      </c>
+      <c r="E13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>C17738</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C14" t="s">
+        <v>177</v>
+      </c>
+      <c r="D14" t="s">
+        <v>184</v>
+      </c>
+      <c r="E14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>C22843</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>20</v>
       </c>
-      <c r="H5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I5" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J5" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K5" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L5" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M5" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="3">
-        <v>3</v>
-      </c>
-      <c r="D6" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E6" s="3">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I6" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J6" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K6" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L6" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M6" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
-      <c r="B7" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="3">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E7" s="3">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L7" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M7" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="5" t="s">
+      <c r="B15" t="s">
+        <v>185</v>
+      </c>
+      <c r="C15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D15" t="s">
+        <v>186</v>
+      </c>
+      <c r="E15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>C22950</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" t="s">
+        <v>188</v>
+      </c>
+      <c r="C16" t="s">
+        <v>177</v>
+      </c>
+      <c r="D16" t="s">
+        <v>189</v>
+      </c>
+      <c r="E16" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v>C23186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C17" t="s">
+        <v>177</v>
+      </c>
+      <c r="D17" t="s">
+        <v>191</v>
+      </c>
+      <c r="E17" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v>C23162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>192</v>
+      </c>
+      <c r="B18" t="s">
+        <v>193</v>
+      </c>
+      <c r="C18" t="s">
+        <v>194</v>
+      </c>
+      <c r="D18" t="s">
+        <v>195</v>
+      </c>
+      <c r="E18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="0"/>
+        <v>C84256</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="3">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E8" s="3">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K8" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L8" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M8" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="C9" s="3">
-        <f>SUM(C2:C8)</f>
-        <v>15</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="3">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E10" s="3">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="3"/>
-        <v>40</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K10" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L10" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M10" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E11" s="3">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K11" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L11" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M11" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="3">
-        <v>1</v>
-      </c>
-      <c r="D12" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E12" s="3">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="3">
-        <v>2</v>
-      </c>
-      <c r="D13" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E13" s="3">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L13" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
-      <c r="B14" s="5">
-        <v>20</v>
-      </c>
-      <c r="C14" s="3">
-        <v>10</v>
-      </c>
-      <c r="D14" s="3">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="E14" s="3">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="3"/>
-        <v>100</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K14" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L14" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="5">
-        <v>51</v>
-      </c>
-      <c r="C15" s="3">
-        <v>5</v>
-      </c>
-      <c r="D15" s="3">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="E15" s="3">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K15" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L15" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M15" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="3">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E16" s="3">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L16" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C17" s="3">
-        <f>SUM(C10:C16)</f>
-        <v>24</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="3">
-        <v>38</v>
-      </c>
-      <c r="D18" s="3">
-        <f t="shared" si="0"/>
-        <v>76</v>
-      </c>
-      <c r="E18" s="3">
-        <f t="shared" si="1"/>
-        <v>228</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="3"/>
-        <v>380</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K18" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L18" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M18" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="3">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E19" s="3">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K19" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L19" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M19" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>196</v>
+      </c>
+      <c r="C19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D19" t="s">
+        <v>198</v>
+      </c>
+      <c r="E19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="0"/>
+        <v>C135336</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="3">
-        <v>1</v>
-      </c>
-      <c r="D20" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E20" s="3">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K20" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L20" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M20" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="3">
-        <v>1</v>
-      </c>
-      <c r="D21" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E21" s="3">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J21" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K21" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L21" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M21" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" s="3">
-        <v>1</v>
-      </c>
-      <c r="D22" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E22" s="3">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K22" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L22" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M22" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+      <c r="B20" t="s">
+        <v>200</v>
+      </c>
+      <c r="C20" t="s">
+        <v>201</v>
+      </c>
+      <c r="D20" t="s">
+        <v>202</v>
+      </c>
+      <c r="E20" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>230</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="0"/>
+        <v>C720477</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>203</v>
+      </c>
+      <c r="B21" t="s">
+        <v>204</v>
+      </c>
+      <c r="C21" t="s">
+        <v>205</v>
+      </c>
+      <c r="D21" t="s">
+        <v>206</v>
+      </c>
+      <c r="E21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="0"/>
+        <v>C529355</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>207</v>
+      </c>
+      <c r="B22" t="s">
+        <v>208</v>
+      </c>
+      <c r="C22" t="s">
+        <v>209</v>
+      </c>
+      <c r="D22" t="s">
+        <v>210</v>
+      </c>
+      <c r="E22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="0"/>
+        <v>C2940549</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="3">
-        <v>38</v>
-      </c>
-      <c r="D23" s="3">
-        <f t="shared" si="0"/>
-        <v>76</v>
-      </c>
-      <c r="E23" s="3">
-        <f t="shared" si="1"/>
-        <v>228</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="3"/>
-        <v>380</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J23" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K23" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L23" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M23" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+      <c r="B23" t="s">
+        <v>212</v>
+      </c>
+      <c r="C23" t="s">
+        <v>213</v>
+      </c>
+      <c r="D23" t="s">
+        <v>214</v>
+      </c>
+      <c r="E23" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="0"/>
+        <v>C2988369</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="3">
-        <v>38</v>
-      </c>
-      <c r="D24" s="3">
-        <f t="shared" si="0"/>
-        <v>76</v>
-      </c>
-      <c r="E24" s="3">
-        <f t="shared" si="1"/>
-        <v>228</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="3"/>
-        <v>380</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I24" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K24" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L24" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M24" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>74</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="3">
-        <v>2</v>
-      </c>
-      <c r="D25" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E25" s="3">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J25" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K25" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L25" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M25" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>75</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="3">
-        <v>1</v>
-      </c>
-      <c r="D26" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E26" s="3">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J26" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K26" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L26" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M26" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>76</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="3">
-        <v>1</v>
-      </c>
-      <c r="D27" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E27" s="3">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I27" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J27" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K27" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L27" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M27" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="3">
-        <v>2</v>
-      </c>
-      <c r="D28" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E28" s="3">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I28" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J28" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K28" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L28" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M28" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="3">
-        <v>1</v>
-      </c>
-      <c r="D29" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E29" s="3">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I29" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J29" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K29" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L29" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M29" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>78</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="3">
-        <v>2</v>
-      </c>
-      <c r="D30" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E30" s="3">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="H30">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I30" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J30" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K30" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L30" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M30" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="3">
-        <v>1</v>
-      </c>
-      <c r="D31" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E31" s="3">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="H31">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I31" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J31" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K31" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L31" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M31" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C32" s="3">
-        <f>C9+C17+SUM(C18:C31)</f>
-        <v>167</v>
-      </c>
-      <c r="I32" s="4">
-        <f>SUM(I2:I31)</f>
-        <v>1.786</v>
-      </c>
-      <c r="J32" s="4">
-        <f t="shared" ref="J32:L32" si="6">SUM(J2:J31)</f>
-        <v>3.5720000000000001</v>
-      </c>
-      <c r="K32" s="4">
-        <f t="shared" si="6"/>
-        <v>10.716000000000001</v>
-      </c>
-      <c r="L32" s="4">
-        <f t="shared" si="6"/>
-        <v>17.86</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>8</v>
-      </c>
-      <c r="C49" s="3">
-        <v>38</v>
-      </c>
-      <c r="D49" s="3">
-        <f t="shared" ref="D49:D62" si="7">2*C49</f>
-        <v>76</v>
-      </c>
-      <c r="E49" s="3">
-        <f t="shared" ref="E49:E62" si="8">D49*$P$2</f>
-        <v>228</v>
-      </c>
-      <c r="F49">
-        <f t="shared" ref="F49:F62" si="9">D49*5</f>
-        <v>380</v>
-      </c>
-      <c r="H49">
-        <f t="shared" ref="H49:H62" si="10">G49*17.86</f>
-        <v>0</v>
-      </c>
-      <c r="I49" s="4">
-        <f t="shared" ref="I49:I62" si="11">IF($M49, $H49*C49, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="J49" s="4">
-        <f t="shared" ref="J49:J62" si="12">IF($M49, $H49*D49, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="K49" s="4">
-        <f t="shared" ref="K49:K62" si="13">IF($M49, $H49*E49, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="L49" s="4">
-        <f t="shared" ref="L49:L62" si="14">IF($M49, $H49*F49, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="M49" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>11</v>
-      </c>
-      <c r="C50" s="3">
-        <v>24</v>
-      </c>
-      <c r="D50" s="3">
-        <f t="shared" si="7"/>
-        <v>48</v>
-      </c>
-      <c r="E50" s="3">
-        <f t="shared" si="8"/>
-        <v>144</v>
-      </c>
-      <c r="F50">
-        <f t="shared" si="9"/>
-        <v>240</v>
-      </c>
-      <c r="G50">
-        <v>2.2000000000000001E-3</v>
-      </c>
-      <c r="H50">
-        <f t="shared" si="10"/>
-        <v>3.9292000000000001E-2</v>
-      </c>
-      <c r="I50" s="4">
-        <f t="shared" si="11"/>
-        <v>0.94300800000000007</v>
-      </c>
-      <c r="J50" s="4">
-        <f t="shared" si="12"/>
-        <v>1.8860160000000001</v>
-      </c>
-      <c r="K50" s="4">
-        <f t="shared" si="13"/>
-        <v>5.658048</v>
-      </c>
-      <c r="L50" s="4">
-        <f t="shared" si="14"/>
-        <v>9.4300800000000002</v>
-      </c>
-      <c r="M50" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51" s="3">
-        <v>2</v>
-      </c>
-      <c r="D51" s="3">
-        <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
-      <c r="E51" s="3">
-        <f t="shared" si="8"/>
-        <v>12</v>
-      </c>
-      <c r="F51">
-        <f t="shared" si="9"/>
-        <v>20</v>
-      </c>
-      <c r="G51">
-        <v>0.2</v>
-      </c>
-      <c r="H51">
-        <f t="shared" si="10"/>
-        <v>3.5720000000000001</v>
-      </c>
-      <c r="I51" s="4">
-        <f t="shared" si="11"/>
-        <v>7.1440000000000001</v>
-      </c>
-      <c r="J51" s="4">
-        <f t="shared" si="12"/>
-        <v>14.288</v>
-      </c>
-      <c r="K51" s="4">
-        <f t="shared" si="13"/>
-        <v>42.864000000000004</v>
-      </c>
-      <c r="L51" s="4">
-        <f t="shared" si="14"/>
-        <v>71.44</v>
-      </c>
-      <c r="M51" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q51" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>13</v>
-      </c>
-      <c r="C52" s="3">
-        <v>38</v>
-      </c>
-      <c r="D52" s="3">
-        <f t="shared" si="7"/>
-        <v>76</v>
-      </c>
-      <c r="E52" s="3">
-        <f t="shared" si="8"/>
-        <v>228</v>
-      </c>
-      <c r="F52">
-        <f t="shared" si="9"/>
-        <v>380</v>
-      </c>
-      <c r="G52">
-        <v>0.26</v>
-      </c>
-      <c r="H52">
-        <f t="shared" si="10"/>
-        <v>4.6436000000000002</v>
-      </c>
-      <c r="I52" s="4">
-        <f t="shared" si="11"/>
-        <v>176.45680000000002</v>
-      </c>
-      <c r="J52" s="4">
-        <f t="shared" si="12"/>
-        <v>352.91360000000003</v>
-      </c>
-      <c r="K52" s="4">
-        <f t="shared" si="13"/>
-        <v>1058.7408</v>
-      </c>
-      <c r="L52" s="4">
-        <f t="shared" si="14"/>
-        <v>1764.568</v>
-      </c>
-      <c r="M52" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="S52" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>14</v>
-      </c>
-      <c r="C53" s="3">
-        <v>38</v>
-      </c>
-      <c r="D53" s="3">
-        <f t="shared" si="7"/>
-        <v>76</v>
-      </c>
-      <c r="E53" s="3">
-        <f t="shared" si="8"/>
-        <v>228</v>
-      </c>
-      <c r="F53">
-        <f t="shared" si="9"/>
-        <v>380</v>
-      </c>
-      <c r="H53">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I53" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J53" s="4">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="K53" s="4">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="L53" s="4">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="M53" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>15</v>
-      </c>
-      <c r="C54" s="3">
-        <v>3</v>
-      </c>
-      <c r="D54" s="3">
-        <f t="shared" si="7"/>
-        <v>6</v>
-      </c>
-      <c r="E54" s="3">
-        <f t="shared" si="8"/>
-        <v>18</v>
-      </c>
-      <c r="F54">
-        <f t="shared" si="9"/>
-        <v>30</v>
-      </c>
-      <c r="H54">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I54" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J54" s="4">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="K54" s="4">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="L54" s="4">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="M54" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>16</v>
-      </c>
-      <c r="C55" s="3">
-        <v>1</v>
-      </c>
-      <c r="D55" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E55" s="3">
-        <f t="shared" si="8"/>
-        <v>6</v>
-      </c>
-      <c r="F55">
-        <f t="shared" si="9"/>
-        <v>10</v>
-      </c>
-      <c r="H55">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I55" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J55" s="4">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="K55" s="4">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="L55" s="4">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="M55" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>9</v>
-      </c>
-      <c r="C56" s="3">
-        <v>1</v>
-      </c>
-      <c r="D56" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E56" s="3">
-        <f t="shared" si="8"/>
-        <v>6</v>
-      </c>
-      <c r="F56">
-        <f t="shared" si="9"/>
-        <v>10</v>
-      </c>
-      <c r="G56">
-        <v>1.7565</v>
-      </c>
-      <c r="H56">
-        <f t="shared" si="10"/>
-        <v>31.371089999999999</v>
-      </c>
-      <c r="I56" s="4">
-        <f t="shared" si="11"/>
-        <v>31.371089999999999</v>
-      </c>
-      <c r="J56" s="4">
-        <f t="shared" si="12"/>
-        <v>62.742179999999998</v>
-      </c>
-      <c r="K56" s="4">
-        <f t="shared" si="13"/>
-        <v>188.22654</v>
-      </c>
-      <c r="L56" s="4">
-        <f t="shared" si="14"/>
-        <v>313.71089999999998</v>
-      </c>
-      <c r="M56" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>10</v>
-      </c>
-      <c r="C57" s="3">
-        <v>1</v>
-      </c>
-      <c r="D57" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E57" s="3">
-        <f t="shared" si="8"/>
-        <v>6</v>
-      </c>
-      <c r="F57">
-        <f t="shared" si="9"/>
-        <v>10</v>
-      </c>
-      <c r="G57">
-        <v>0.95099999999999996</v>
-      </c>
-      <c r="H57">
-        <f t="shared" si="10"/>
-        <v>16.984859999999998</v>
-      </c>
-      <c r="I57" s="4">
-        <f t="shared" si="11"/>
-        <v>16.984859999999998</v>
-      </c>
-      <c r="J57" s="4">
-        <f t="shared" si="12"/>
-        <v>33.969719999999995</v>
-      </c>
-      <c r="K57" s="4">
-        <f t="shared" si="13"/>
-        <v>101.90915999999999</v>
-      </c>
-      <c r="L57" s="4">
-        <f t="shared" si="14"/>
-        <v>169.84859999999998</v>
-      </c>
-      <c r="M57" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>17</v>
-      </c>
-      <c r="C58" s="3">
-        <v>2</v>
-      </c>
-      <c r="D58" s="3">
-        <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
-      <c r="E58" s="3">
-        <f t="shared" si="8"/>
-        <v>12</v>
-      </c>
-      <c r="F58">
-        <f t="shared" si="9"/>
-        <v>20</v>
-      </c>
-      <c r="G58">
-        <v>6.0199999999999997E-2</v>
-      </c>
-      <c r="H58">
-        <f t="shared" si="10"/>
-        <v>1.0751719999999998</v>
-      </c>
-      <c r="I58" s="4">
-        <f t="shared" si="11"/>
-        <v>2.1503439999999996</v>
-      </c>
-      <c r="J58" s="4">
-        <f t="shared" si="12"/>
-        <v>4.3006879999999992</v>
-      </c>
-      <c r="K58" s="4">
-        <f t="shared" si="13"/>
-        <v>12.902063999999998</v>
-      </c>
-      <c r="L58" s="4">
-        <f t="shared" si="14"/>
-        <v>21.503439999999998</v>
-      </c>
-      <c r="M58" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>18</v>
-      </c>
-      <c r="C59" s="3">
-        <v>1</v>
-      </c>
-      <c r="D59" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E59" s="3">
-        <f t="shared" si="8"/>
-        <v>6</v>
-      </c>
-      <c r="F59">
-        <f t="shared" si="9"/>
-        <v>10</v>
-      </c>
-      <c r="G59">
-        <v>0.1704</v>
-      </c>
-      <c r="H59">
-        <f t="shared" si="10"/>
-        <v>3.0433439999999998</v>
-      </c>
-      <c r="I59" s="4">
-        <f t="shared" si="11"/>
-        <v>3.0433439999999998</v>
-      </c>
-      <c r="J59" s="4">
-        <f t="shared" si="12"/>
-        <v>6.0866879999999997</v>
-      </c>
-      <c r="K59" s="4">
-        <f t="shared" si="13"/>
-        <v>18.260064</v>
-      </c>
-      <c r="L59" s="4">
-        <f t="shared" si="14"/>
-        <v>30.433439999999997</v>
-      </c>
-      <c r="M59" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>19</v>
-      </c>
-      <c r="C60" s="3">
-        <v>2</v>
-      </c>
-      <c r="D60" s="3">
-        <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
-      <c r="E60" s="3">
-        <f t="shared" si="8"/>
-        <v>12</v>
-      </c>
-      <c r="F60">
-        <f t="shared" si="9"/>
-        <v>20</v>
-      </c>
-      <c r="G60">
-        <v>7.8600000000000003E-2</v>
-      </c>
-      <c r="H60">
-        <f t="shared" si="10"/>
-        <v>1.403796</v>
-      </c>
-      <c r="I60" s="4">
-        <f t="shared" si="11"/>
-        <v>2.8075920000000001</v>
-      </c>
-      <c r="J60" s="4">
-        <f t="shared" si="12"/>
-        <v>5.6151840000000002</v>
-      </c>
-      <c r="K60" s="4">
-        <f t="shared" si="13"/>
-        <v>16.845552000000001</v>
-      </c>
-      <c r="L60" s="4">
-        <f t="shared" si="14"/>
-        <v>28.07592</v>
-      </c>
-      <c r="M60" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>20</v>
-      </c>
-      <c r="C61" s="3">
-        <v>1</v>
-      </c>
-      <c r="D61" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E61" s="3">
-        <f t="shared" si="8"/>
-        <v>6</v>
-      </c>
-      <c r="F61">
-        <f t="shared" si="9"/>
-        <v>10</v>
-      </c>
-      <c r="G61">
-        <v>6.6500000000000004E-2</v>
-      </c>
-      <c r="H61">
-        <f t="shared" si="10"/>
-        <v>1.1876900000000001</v>
-      </c>
-      <c r="I61" s="4">
-        <f t="shared" si="11"/>
-        <v>1.1876900000000001</v>
-      </c>
-      <c r="J61" s="4">
-        <f t="shared" si="12"/>
-        <v>2.3753800000000003</v>
-      </c>
-      <c r="K61" s="4">
-        <f t="shared" si="13"/>
-        <v>7.1261400000000013</v>
-      </c>
-      <c r="L61" s="4">
-        <f t="shared" si="14"/>
-        <v>11.876900000000001</v>
-      </c>
-      <c r="M61" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>50</v>
-      </c>
-      <c r="C62" s="3">
-        <v>2</v>
-      </c>
-      <c r="D62" s="3">
-        <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
-      <c r="E62" s="3">
-        <f t="shared" si="8"/>
-        <v>12</v>
-      </c>
-      <c r="F62">
-        <f t="shared" si="9"/>
-        <v>20</v>
-      </c>
-      <c r="H62">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I62" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J62" s="4">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="K62" s="4">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="L62" s="4">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>29</v>
-      </c>
-      <c r="I63" s="4">
-        <f>SUM(I2:I61)</f>
-        <v>245.66072800000001</v>
-      </c>
-      <c r="J63" s="4">
-        <f>SUM(J2:J61)</f>
-        <v>491.32145600000001</v>
-      </c>
-      <c r="K63" s="4">
-        <f>SUM(K2:K61)</f>
-        <v>1473.9643680000004</v>
-      </c>
-      <c r="L63" s="4">
-        <f>SUM(L2:L61)</f>
-        <v>2456.6072799999997</v>
+        <v>114</v>
+      </c>
+      <c r="B24" t="s">
+        <v>215</v>
+      </c>
+      <c r="C24" t="s">
+        <v>216</v>
+      </c>
+      <c r="D24" t="s">
+        <v>217</v>
+      </c>
+      <c r="E24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="0"/>
+        <v>C29780639</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A10:A16"/>
-    <mergeCell ref="A21:A22"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding Panels to PCB
</commit_message>
<xml_diff>
--- a/PartsList.xlsx
+++ b/PartsList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matja\Documents\Projects\PCBs\Keyboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE310610-1642-4D72-94A3-B1FD26362629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89903664-EBFD-4C7E-9804-02D1DAC955E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="3" xr2:uid="{FE2F31EC-1493-4486-83E7-300EEFA8040E}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="233">
   <si>
     <t>Name</t>
   </si>
@@ -732,6 +732,12 @@
   </si>
   <si>
     <t>C720477</t>
+  </si>
+  <si>
+    <t>C20798</t>
+  </si>
+  <si>
+    <t>No Stock of 1</t>
   </si>
 </sst>
 </file>
@@ -5931,10 +5937,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04496EBE-FF58-4432-A51C-6782192DBBAD}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6313,7 +6319,7 @@
         <v>C23186</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>101</v>
       </c>
@@ -6334,7 +6340,7 @@
         <v>C23162</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>192</v>
       </c>
@@ -6358,7 +6364,7 @@
         <v>C84256</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -6372,14 +6378,20 @@
         <v>198</v>
       </c>
       <c r="E19" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>231</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
-        <v>C135336</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>C20798</v>
+      </c>
+      <c r="I19" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>199</v>
       </c>
@@ -6403,7 +6415,7 @@
         <v>C720477</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>203</v>
       </c>
@@ -6424,7 +6436,7 @@
         <v>C529355</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>207</v>
       </c>
@@ -6445,7 +6457,7 @@
         <v>C2940549</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>211</v>
       </c>
@@ -6466,7 +6478,7 @@
         <v>C2988369</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>114</v>
       </c>

</xml_diff>